<commit_message>
New benchmark results for TPCH queries + Consistent formatting for Benchmarks
</commit_message>
<xml_diff>
--- a/docs/benchmarks/tpch_queries.xlsx
+++ b/docs/benchmarks/tpch_queries.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tpch_standard" sheetId="1" r:id="rId1"/>
+    <sheet name="tpch_standard_improvement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
   <si>
     <t>Dataset</t>
   </si>
@@ -101,11 +102,35 @@
   <si>
     <t>K3Optimizer -O3</t>
   </si>
+  <si>
+    <t>Scala</t>
+  </si>
+  <si>
+    <t>LMS</t>
+  </si>
+  <si>
+    <t>Scala-legacy</t>
+  </si>
+  <si>
+    <t>LMS-legacy</t>
+  </si>
+  <si>
+    <t>tpch7</t>
+  </si>
+  <si>
+    <t>tpch8</t>
+  </si>
+  <si>
+    <t>tpch9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -148,7 +173,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -164,11 +189,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -176,6 +204,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -183,6 +212,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,11 +526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="140420840"/>
-        <c:axId val="140427768"/>
+        <c:axId val="546475416"/>
+        <c:axId val="100931704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="140420840"/>
+        <c:axId val="546475416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,13 +552,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140427768"/>
+        <c:crossAx val="100931704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -536,7 +565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140427768"/>
+        <c:axId val="100931704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,16 +588,628 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140420840"/>
+        <c:crossAx val="546475416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$A$3:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tpch9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tpch11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tpch13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_standard_improvement!$G$19:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.891304347826087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.07608695652174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.192660550458716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.243589743589744</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89247311827957</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.552173913043478</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.363117870722433</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.943396226415094</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.188976377952756</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.08421052631579</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.988372093023256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$A$3:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tpch9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tpch11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tpch13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_standard_improvement!$L$19:$L$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala-legacy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0220264317180617"/>
+                  <c:y val="0.712781954887218"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0229074889867841"/>
+                  <c:y val="0.616541353383459"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$A$3:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tpch9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tpch11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tpch13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_standard_improvement!$Q$19:$Q$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.233076086956522</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.52616666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.545260869565217</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.997724770642202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.39996153846154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.84141935483871</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.96521739130434</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.784935361216729</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.452077568134172</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.882850393700787</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>69.50175</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.715557894736842</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.43309302325581</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-legacy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0193832599118943"/>
+                  <c:y val="0.673684210526316"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_standard_improvement!$A$3:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tpch9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tpch11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tpch13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_standard_improvement!$V$19:$V$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.019114130434783</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.19675</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.057521739130434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.913357798165137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.12476923076923</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.854333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.19565217391303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.731479087452471</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.67738784067086</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.449062992125984</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.8664375</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.090105263157894</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.443872093023256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="551057912"/>
+        <c:axId val="551061048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="551057912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="551061048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="551061048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="19.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="551057912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -606,6 +1247,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -947,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
@@ -1995,7 +2671,1306 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="D3">
+        <v>6.9109999999999996</v>
+      </c>
+      <c r="E3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="F3">
+        <v>6.3E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="H3">
+        <v>1.284</v>
+      </c>
+      <c r="I3">
+        <v>1.694</v>
+      </c>
+      <c r="J3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K3">
+        <v>6.3E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.184</v>
+      </c>
+      <c r="M3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="N3">
+        <v>5.3819999999999997</v>
+      </c>
+      <c r="O3">
+        <v>0.191825</v>
+      </c>
+      <c r="P3">
+        <v>0.17455999999999999</v>
+      </c>
+      <c r="Q3">
+        <v>0.41088599999999997</v>
+      </c>
+      <c r="R3">
+        <v>46.308</v>
+      </c>
+      <c r="S3">
+        <v>1.552</v>
+      </c>
+      <c r="T3">
+        <v>0.151417</v>
+      </c>
+      <c r="U3">
+        <v>0.12706400000000001</v>
+      </c>
+      <c r="V3">
+        <v>0.18751699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D4">
+        <v>1.054</v>
+      </c>
+      <c r="E4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G4">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H4">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="J4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M4">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="N4">
+        <v>3.9630000000000001</v>
+      </c>
+      <c r="O4">
+        <v>0.105998</v>
+      </c>
+      <c r="P4">
+        <v>9.3771999999999994E-2</v>
+      </c>
+      <c r="Q4">
+        <v>0.13831399999999999</v>
+      </c>
+      <c r="R4">
+        <v>98.912999999999997</v>
+      </c>
+      <c r="S4">
+        <v>1.5349999999999999</v>
+      </c>
+      <c r="T4">
+        <v>5.5120000000000002E-2</v>
+      </c>
+      <c r="U4">
+        <v>4.9498E-2</v>
+      </c>
+      <c r="V4">
+        <v>6.2361E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="C5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.09</v>
+      </c>
+      <c r="F5">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G5">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.434</v>
+      </c>
+      <c r="J5">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="K5">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="M5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="N5">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="O5">
+        <v>0.233066</v>
+      </c>
+      <c r="P5">
+        <v>0.19775999999999999</v>
+      </c>
+      <c r="Q5">
+        <v>0.32616400000000001</v>
+      </c>
+      <c r="R5">
+        <v>32.991</v>
+      </c>
+      <c r="S5">
+        <v>0.84</v>
+      </c>
+      <c r="T5">
+        <v>0.20478399999999999</v>
+      </c>
+      <c r="U5">
+        <v>0.16816800000000001</v>
+      </c>
+      <c r="V5">
+        <v>0.28129199999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.09</v>
+      </c>
+      <c r="F6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.13</v>
+      </c>
+      <c r="H6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="J6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="K6">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.109</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0.52</v>
+      </c>
+      <c r="O6">
+        <v>0.19809599999999999</v>
+      </c>
+      <c r="P6">
+        <v>0.14992</v>
+      </c>
+      <c r="Q6">
+        <v>0.217752</v>
+      </c>
+      <c r="R6">
+        <v>19.047999999999998</v>
+      </c>
+      <c r="S6">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="T6">
+        <v>0.18748999999999999</v>
+      </c>
+      <c r="U6">
+        <v>0.15110100000000001</v>
+      </c>
+      <c r="V6">
+        <v>0.20855599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="C7">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="D7">
+        <v>1.228</v>
+      </c>
+      <c r="E7">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.107</v>
+      </c>
+      <c r="G7">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="I7">
+        <v>1.091</v>
+      </c>
+      <c r="J7">
+        <v>0.124</v>
+      </c>
+      <c r="K7">
+        <v>0.113</v>
+      </c>
+      <c r="L7">
+        <v>0.156</v>
+      </c>
+      <c r="M7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="N7">
+        <v>3.7320000000000002</v>
+      </c>
+      <c r="O7">
+        <v>0.75559699999999996</v>
+      </c>
+      <c r="P7">
+        <v>0.63960600000000001</v>
+      </c>
+      <c r="Q7">
+        <v>2.0903939999999999</v>
+      </c>
+      <c r="R7">
+        <v>67.477999999999994</v>
+      </c>
+      <c r="S7">
+        <v>1.837</v>
+      </c>
+      <c r="T7">
+        <v>0.36193500000000001</v>
+      </c>
+      <c r="U7">
+        <v>0.32459100000000002</v>
+      </c>
+      <c r="V7">
+        <v>1.2674639999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="E8">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="F8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="J8">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K8">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="L8">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="O8">
+        <v>0.151175</v>
+      </c>
+      <c r="P8">
+        <v>0.123173</v>
+      </c>
+      <c r="Q8">
+        <v>0.17125199999999999</v>
+      </c>
+      <c r="R8">
+        <v>12.449</v>
+      </c>
+      <c r="S8">
+        <v>0.37</v>
+      </c>
+      <c r="T8">
+        <v>0.13774500000000001</v>
+      </c>
+      <c r="U8">
+        <v>0.12443899999999999</v>
+      </c>
+      <c r="V8">
+        <v>0.172453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>4.6920000000000002</v>
+      </c>
+      <c r="C9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D9">
+        <v>22.004999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="F9">
+        <v>0.15</v>
+      </c>
+      <c r="G9">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="H9">
+        <v>4.7519999999999998</v>
+      </c>
+      <c r="I9">
+        <v>3.26</v>
+      </c>
+      <c r="J9">
+        <v>0.12</v>
+      </c>
+      <c r="K9">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="L9">
+        <v>0.23</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>9.6489999999999991</v>
+      </c>
+      <c r="O9">
+        <v>14.715999999999999</v>
+      </c>
+      <c r="P9">
+        <v>14.337999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>17.242000000000001</v>
+      </c>
+      <c r="R9">
+        <v>111.57</v>
+      </c>
+      <c r="S9">
+        <v>4.5919999999999996</v>
+      </c>
+      <c r="T9">
+        <v>8.1180000000000003</v>
+      </c>
+      <c r="U9">
+        <v>7.9850000000000003</v>
+      </c>
+      <c r="V9">
+        <v>16.145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>12.432</v>
+      </c>
+      <c r="C10">
+        <v>1.242</v>
+      </c>
+      <c r="D10">
+        <v>13.750999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="H10">
+        <v>4.6980000000000004</v>
+      </c>
+      <c r="I10">
+        <v>5.3650000000000002</v>
+      </c>
+      <c r="J10">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.12</v>
+      </c>
+      <c r="L10">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="M10">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="N10">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="O10">
+        <v>2.4744980000000001</v>
+      </c>
+      <c r="P10">
+        <v>2.322346</v>
+      </c>
+      <c r="Q10">
+        <v>3.5688759999999999</v>
+      </c>
+      <c r="R10">
+        <v>238.273</v>
+      </c>
+      <c r="S10">
+        <v>6.069</v>
+      </c>
+      <c r="T10">
+        <v>1.387553</v>
+      </c>
+      <c r="U10">
+        <v>1.237374</v>
+      </c>
+      <c r="V10">
+        <v>1.962758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>2.2629999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.37</v>
+      </c>
+      <c r="D11">
+        <v>2.13</v>
+      </c>
+      <c r="E11">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.45</v>
+      </c>
+      <c r="H11">
+        <v>1.4450000000000001</v>
+      </c>
+      <c r="I11">
+        <v>1.849</v>
+      </c>
+      <c r="J11">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="K11">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="L11">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="M11">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="N11">
+        <v>10.483000000000001</v>
+      </c>
+      <c r="O11">
+        <v>1.8676360000000001</v>
+      </c>
+      <c r="P11">
+        <v>1.780176</v>
+      </c>
+      <c r="Q11">
+        <v>2.600641</v>
+      </c>
+      <c r="R11">
+        <v>122.411</v>
+      </c>
+      <c r="S11">
+        <v>2.9609999999999999</v>
+      </c>
+      <c r="T11">
+        <v>0.853383</v>
+      </c>
+      <c r="U11">
+        <v>0.789412</v>
+      </c>
+      <c r="V11">
+        <v>1.2771140000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.217</v>
+      </c>
+      <c r="C12">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="D12">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="F12">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.151</v>
+      </c>
+      <c r="H12">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I12">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="J12">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="K12">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="L12">
+        <v>0.127</v>
+      </c>
+      <c r="M12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N12">
+        <v>2.077</v>
+      </c>
+      <c r="O12">
+        <v>0.24121600000000001</v>
+      </c>
+      <c r="P12">
+        <v>0.19203000000000001</v>
+      </c>
+      <c r="Q12">
+        <v>0.62012199999999995</v>
+      </c>
+      <c r="R12">
+        <v>39.914000000000001</v>
+      </c>
+      <c r="S12">
+        <v>1.448</v>
+      </c>
+      <c r="T12">
+        <v>0.2006</v>
+      </c>
+      <c r="U12">
+        <v>0.17055699999999999</v>
+      </c>
+      <c r="V12">
+        <v>0.311031</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0.72</v>
+      </c>
+      <c r="C13">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E13">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.01</v>
+      </c>
+      <c r="G13">
+        <v>0.02</v>
+      </c>
+      <c r="H13">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="J13">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K13">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L13">
+        <v>1.6E-2</v>
+      </c>
+      <c r="M13">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="N13">
+        <v>5.52</v>
+      </c>
+      <c r="O13">
+        <v>0.28439700000000001</v>
+      </c>
+      <c r="P13">
+        <v>0.27990799999999999</v>
+      </c>
+      <c r="Q13">
+        <v>1.112028</v>
+      </c>
+      <c r="R13">
+        <v>62.048000000000002</v>
+      </c>
+      <c r="S13">
+        <v>0.877</v>
+      </c>
+      <c r="T13">
+        <v>0.10356700000000001</v>
+      </c>
+      <c r="U13">
+        <v>8.4607000000000002E-2</v>
+      </c>
+      <c r="V13">
+        <v>0.25386300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C14">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="E14">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F14">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="H14">
+        <v>0.21</v>
+      </c>
+      <c r="I14">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="J14">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K14">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L14">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="M14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N14">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="O14">
+        <v>0.20944599999999999</v>
+      </c>
+      <c r="P14">
+        <v>0.16055900000000001</v>
+      </c>
+      <c r="Q14">
+        <v>0.25797799999999999</v>
+      </c>
+      <c r="R14">
+        <v>27.088999999999999</v>
+      </c>
+      <c r="S14">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="T14">
+        <v>0.18043200000000001</v>
+      </c>
+      <c r="U14">
+        <v>0.14716000000000001</v>
+      </c>
+      <c r="V14">
+        <v>0.19855999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="C15">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="D15">
+        <v>0.498</v>
+      </c>
+      <c r="E15">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>3.1E-2</v>
+      </c>
+      <c r="G15">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H15">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="I15">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="J15">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L15">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="M15">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="N15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O15">
+        <v>1.1658219999999999</v>
+      </c>
+      <c r="P15">
+        <v>1.0913580000000001</v>
+      </c>
+      <c r="Q15">
+        <v>1.5852459999999999</v>
+      </c>
+      <c r="R15">
+        <v>45.351999999999997</v>
+      </c>
+      <c r="S15">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="T15">
+        <v>0.238733</v>
+      </c>
+      <c r="U15">
+        <v>0.21390600000000001</v>
+      </c>
+      <c r="V15">
+        <v>0.46817300000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>0.32</v>
+      </c>
+      <c r="C16">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="E16">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F16">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G16">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="H16">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="J16">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="K16">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="L16">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="O16">
+        <v>0.15112999999999999</v>
+      </c>
+      <c r="P16">
+        <v>0.122102</v>
+      </c>
+      <c r="Q16">
+        <v>0.19846900000000001</v>
+      </c>
+      <c r="R16">
+        <v>27.437999999999999</v>
+      </c>
+      <c r="S16">
+        <v>0.59</v>
+      </c>
+      <c r="T16">
+        <v>0.152891</v>
+      </c>
+      <c r="U16">
+        <v>0.12567999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0.174203</v>
+      </c>
+    </row>
+    <row r="19" spans="7:22">
+      <c r="G19" s="1">
+        <f>G3/$L3</f>
+        <v>2.8913043478260874</v>
+      </c>
+      <c r="L19" s="1">
+        <f>L3/$L3</f>
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>Q3/$L3</f>
+        <v>2.2330760869565216</v>
+      </c>
+      <c r="V19" s="1">
+        <f>V3/$L3</f>
+        <v>1.0191141304347826</v>
+      </c>
+    </row>
+    <row r="20" spans="7:22">
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G31" si="0">G4/$L4</f>
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" ref="L20:L31" si="1">L4/$L4</f>
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" ref="Q20:Q31" si="2">Q4/$L4</f>
+        <v>11.526166666666667</v>
+      </c>
+      <c r="V20" s="1">
+        <f t="shared" ref="V20:V31" si="3">V4/$L4</f>
+        <v>5.1967499999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="7:22">
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0760869565217392</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5452608695652175</v>
+      </c>
+      <c r="V21" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0575217391304346</v>
+      </c>
+    </row>
+    <row r="22" spans="7:22">
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1926605504587156</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9977247706422019</v>
+      </c>
+      <c r="V22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.9133577981651375</v>
+      </c>
+    </row>
+    <row r="23" spans="7:22">
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2435897435897436</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="2"/>
+        <v>13.399961538461538</v>
+      </c>
+      <c r="V23" s="1">
+        <f t="shared" si="3"/>
+        <v>8.1247692307692301</v>
+      </c>
+    </row>
+    <row r="24" spans="7:22">
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89247311827956999</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8414193548387097</v>
+      </c>
+      <c r="V24" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8543333333333334</v>
+      </c>
+    </row>
+    <row r="25" spans="7:22">
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>4.552173913043478</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="2"/>
+        <v>74.96521739130435</v>
+      </c>
+      <c r="V25" s="1">
+        <f t="shared" si="3"/>
+        <v>70.195652173913032</v>
+      </c>
+    </row>
+    <row r="26" spans="7:22">
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3631178707224334</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7849353612167294</v>
+      </c>
+      <c r="V26" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7314790874524713</v>
+      </c>
+    </row>
+    <row r="27" spans="7:22">
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.94339622641509435</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="2"/>
+        <v>5.4520775681341718</v>
+      </c>
+      <c r="V27" s="1">
+        <f t="shared" si="3"/>
+        <v>2.67738784067086</v>
+      </c>
+    </row>
+    <row r="28" spans="7:22">
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1889763779527558</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="2"/>
+        <v>4.882850393700787</v>
+      </c>
+      <c r="V28" s="1">
+        <f t="shared" si="3"/>
+        <v>2.4490629921259841</v>
+      </c>
+    </row>
+    <row r="29" spans="7:22">
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="2"/>
+        <v>69.501750000000001</v>
+      </c>
+      <c r="V29" s="1">
+        <f t="shared" si="3"/>
+        <v>15.8664375</v>
+      </c>
+    </row>
+    <row r="30" spans="7:22">
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0842105263157893</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" si="2"/>
+        <v>2.7155578947368419</v>
+      </c>
+      <c r="V30" s="1">
+        <f t="shared" si="3"/>
+        <v>2.0901052631578945</v>
+      </c>
+    </row>
+    <row r="31" spans="7:22">
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98837209302325602</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="2"/>
+        <v>18.433093023255815</v>
+      </c>
+      <c r="V31" s="1">
+        <f t="shared" si="3"/>
+        <v>5.4438720930232565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
EXPRIMENTS - After inlining HashMap via LMS
</commit_message>
<xml_diff>
--- a/docs/benchmarks/tpch_queries.xlsx
+++ b/docs/benchmarks/tpch_queries.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tpch_standard" sheetId="1" r:id="rId1"/>
     <sheet name="tpch_standard_improvement" sheetId="2" r:id="rId2"/>
+    <sheet name="tpch_big" sheetId="3" r:id="rId3"/>
+    <sheet name="tpch_bigdel" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
   <si>
     <t>Dataset</t>
   </si>
@@ -123,6 +125,15 @@
   <si>
     <t>tpch9</t>
   </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>big_del</t>
+  </si>
+  <si>
+    <t>LMS-Inline-All</t>
+  </si>
 </sst>
 </file>
 
@@ -173,8 +184,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -205,6 +272,34 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -213,6 +308,34 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,11 +649,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="546475416"/>
-        <c:axId val="100931704"/>
+        <c:axId val="172905096"/>
+        <c:axId val="172912040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="546475416"/>
+        <c:axId val="172905096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100931704"/>
+        <c:crossAx val="172912040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100931704"/>
+        <c:axId val="172912040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="546475416"/>
+        <c:crossAx val="172905096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1173,11 +1296,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="551057912"/>
-        <c:axId val="551061048"/>
+        <c:axId val="172293928"/>
+        <c:axId val="172297064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551057912"/>
+        <c:axId val="172293928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,7 +1309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551061048"/>
+        <c:crossAx val="172297064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1194,7 +1317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551061048"/>
+        <c:axId val="172297064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="19.0"/>
@@ -1206,10 +1329,355 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551057912"/>
+        <c:crossAx val="172293928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Inline-All</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$O$13:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.02576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.978810838577116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.986257928118393</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.002959501557632</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.689455388180765</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.951770075243617</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.988817260886725</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.008214849921011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$J$13:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$E$13:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.08112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.008604083729292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.998546511627907</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.998909657320872</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.253765932792584</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.041939065005551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.006578081831338</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99826224328594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="172338808"/>
+        <c:axId val="172341784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="172338808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="172341784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="172341784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Normalized Execution Time (Big Dataset)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="172338808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1221,6 +1689,1093 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Inline-All</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$N$13:$N$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.953418027828191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.005025125628141</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.345588235294117</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.451499118165785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.960677555958862</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.204301075268817</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.043583535108959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.984126984126984</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$I$13:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$D$13:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.813672111312765</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.377721943048576</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.179411764705882</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.14519056261343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.170506912442396</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.186440677966102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.166666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="611170040"/>
+        <c:axId val="611173416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="611170040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="611173416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="611173416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Normalized Compilation Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="611170040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Inline-All</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$M$13:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.481180811808118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.077097505668934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.032967032967033</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.992982456140351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.811320754716981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.117370892018779</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.058823529411764</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$H$13:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$C$13:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.413284132841328</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.412698412698413</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.556776556776557</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.726315789473684</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.218867924528302</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.671361502347418</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.794117647058823</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="611226392"/>
+        <c:axId val="611229368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="611226392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="611229368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="611229368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Normalized CodeGen </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="611226392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_bigdel!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Inline-All</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_bigdel!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_bigdel!$O$13:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.829711435696473</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.979529701366846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.995817843866171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.997885835095137</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.721456692913386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.953546609904213</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.971695663464035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.00742337164751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_bigdel!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_bigdel!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_bigdel!$J$13:$J$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_bigdel!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_bigdel!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_bigdel!$E$13:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.998503740648379</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.010559046446849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.007766861391397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.000156604807767</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.358267716535433</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.026795216928567</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.000389509218385</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.003991060025543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="611275368"/>
+        <c:axId val="611278344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="611275368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="611278344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="611278344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Normalized Execution Time (BigDel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                  <a:t> dataset</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="611275368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1283,6 +2838,142 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2684,8 +4375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3971,6 +5662,1455 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D3">
+        <v>6.3040000000000003</v>
+      </c>
+      <c r="E3">
+        <v>6.7569999999999997</v>
+      </c>
+      <c r="F3">
+        <v>6.6749999999999998</v>
+      </c>
+      <c r="G3">
+        <v>7.5129999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.355</v>
+      </c>
+      <c r="I3">
+        <v>1.653</v>
+      </c>
+      <c r="J3">
+        <v>6.25</v>
+      </c>
+      <c r="K3">
+        <v>6.1779999999999999</v>
+      </c>
+      <c r="L3">
+        <v>7.3179999999999996</v>
+      </c>
+      <c r="M3">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="N3">
+        <v>4.8819999999999997</v>
+      </c>
+      <c r="O3">
+        <v>6.4109999999999996</v>
+      </c>
+      <c r="P3">
+        <v>6.2</v>
+      </c>
+      <c r="Q3">
+        <v>6.8179999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.182</v>
+      </c>
+      <c r="D4">
+        <v>1.645</v>
+      </c>
+      <c r="E4">
+        <v>7.8540000000000001</v>
+      </c>
+      <c r="F4">
+        <v>7.8049999999999997</v>
+      </c>
+      <c r="G4">
+        <v>8.2949999999999999</v>
+      </c>
+      <c r="H4">
+        <v>0.441</v>
+      </c>
+      <c r="I4">
+        <v>1.194</v>
+      </c>
+      <c r="J4">
+        <v>7.7869999999999999</v>
+      </c>
+      <c r="K4">
+        <v>7.6870000000000003</v>
+      </c>
+      <c r="L4">
+        <v>7.9219999999999997</v>
+      </c>
+      <c r="M4">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="N4">
+        <v>3.5880000000000001</v>
+      </c>
+      <c r="O4">
+        <v>7.6219999999999999</v>
+      </c>
+      <c r="P4">
+        <v>7.5709999999999997</v>
+      </c>
+      <c r="Q4">
+        <v>7.9779999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>0.182</v>
+      </c>
+      <c r="C5">
+        <v>0.152</v>
+      </c>
+      <c r="D5">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E5">
+        <v>7.5570000000000004</v>
+      </c>
+      <c r="F5">
+        <v>7.5119999999999996</v>
+      </c>
+      <c r="G5">
+        <v>7.6219999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="I5">
+        <v>0.68</v>
+      </c>
+      <c r="J5">
+        <v>7.5679999999999996</v>
+      </c>
+      <c r="K5">
+        <v>7.53</v>
+      </c>
+      <c r="L5">
+        <v>7.6319999999999997</v>
+      </c>
+      <c r="M5">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="N5">
+        <v>1.595</v>
+      </c>
+      <c r="O5">
+        <v>7.4640000000000004</v>
+      </c>
+      <c r="P5">
+        <v>7.4450000000000003</v>
+      </c>
+      <c r="Q5">
+        <v>7.4980000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>0.31</v>
+      </c>
+      <c r="C6">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.63</v>
+      </c>
+      <c r="E6">
+        <v>6.4130000000000003</v>
+      </c>
+      <c r="F6">
+        <v>6.3639999999999999</v>
+      </c>
+      <c r="G6">
+        <v>6.4630000000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="I6">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="J6">
+        <v>6.42</v>
+      </c>
+      <c r="K6">
+        <v>6.3949999999999996</v>
+      </c>
+      <c r="L6">
+        <v>6.4690000000000003</v>
+      </c>
+      <c r="M6">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="N6">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="O6">
+        <v>6.4390000000000001</v>
+      </c>
+      <c r="P6">
+        <v>6.4050000000000002</v>
+      </c>
+      <c r="Q6">
+        <v>6.6139999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D7">
+        <v>1.893</v>
+      </c>
+      <c r="E7">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="G7">
+        <v>1.5780000000000001</v>
+      </c>
+      <c r="H7">
+        <v>1.325</v>
+      </c>
+      <c r="I7">
+        <v>1.653</v>
+      </c>
+      <c r="J7">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="K7">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="L7">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="M7">
+        <v>1.075</v>
+      </c>
+      <c r="N7">
+        <v>6.5469999999999997</v>
+      </c>
+      <c r="O7">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="P7">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="Q7">
+        <v>1.732</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.185</v>
+      </c>
+      <c r="C8">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="E8">
+        <v>8.4469999999999992</v>
+      </c>
+      <c r="F8">
+        <v>8.1</v>
+      </c>
+      <c r="G8">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="H8">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="J8">
+        <v>8.1069999999999993</v>
+      </c>
+      <c r="K8">
+        <v>8.0109999999999992</v>
+      </c>
+      <c r="L8">
+        <v>8.2859999999999996</v>
+      </c>
+      <c r="M8">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="N8">
+        <v>2.0859999999999999</v>
+      </c>
+      <c r="O8">
+        <v>7.7160000000000002</v>
+      </c>
+      <c r="P8">
+        <v>7.6520000000000001</v>
+      </c>
+      <c r="Q8">
+        <v>7.9329999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.06</v>
+      </c>
+      <c r="D9">
+        <v>0.49</v>
+      </c>
+      <c r="E9">
+        <v>7.6509999999999998</v>
+      </c>
+      <c r="F9">
+        <v>7.569</v>
+      </c>
+      <c r="G9">
+        <v>8.2210000000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.1</v>
+      </c>
+      <c r="I9">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="J9">
+        <v>7.601</v>
+      </c>
+      <c r="K9">
+        <v>7.5540000000000003</v>
+      </c>
+      <c r="L9">
+        <v>7.79</v>
+      </c>
+      <c r="M9">
+        <v>0.111</v>
+      </c>
+      <c r="N9">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="O9">
+        <v>7.516</v>
+      </c>
+      <c r="P9">
+        <v>7.444</v>
+      </c>
+      <c r="Q9">
+        <v>7.6719999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>0.04</v>
+      </c>
+      <c r="C10">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E10">
+        <v>6.319</v>
+      </c>
+      <c r="F10">
+        <v>6.2709999999999999</v>
+      </c>
+      <c r="G10">
+        <v>6.5579999999999998</v>
+      </c>
+      <c r="H10">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.252</v>
+      </c>
+      <c r="J10">
+        <v>6.33</v>
+      </c>
+      <c r="K10">
+        <v>6.29</v>
+      </c>
+      <c r="L10">
+        <v>6.6109999999999998</v>
+      </c>
+      <c r="M10">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="N10">
+        <v>0.248</v>
+      </c>
+      <c r="O10">
+        <v>6.3819999999999997</v>
+      </c>
+      <c r="P10">
+        <v>6.3079999999999998</v>
+      </c>
+      <c r="Q10">
+        <v>6.4619999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="C13">
+        <f>C3/$H3</f>
+        <v>0.41328413284132848</v>
+      </c>
+      <c r="D13">
+        <f>D3/$I3</f>
+        <v>3.8136721113127647</v>
+      </c>
+      <c r="E13">
+        <f>E3/$J3</f>
+        <v>1.0811199999999999</v>
+      </c>
+      <c r="H13">
+        <f>H3/$H3</f>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f>I3/$I3</f>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f>J3/$J3</f>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f>M3/$H3</f>
+        <v>0.48118081180811811</v>
+      </c>
+      <c r="N13">
+        <f>N3/$I3</f>
+        <v>2.953418027828191</v>
+      </c>
+      <c r="O13">
+        <f>O3/$J3</f>
+        <v>1.02576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="C14">
+        <f t="shared" ref="C14:C20" si="0">C4/$H4</f>
+        <v>0.41269841269841268</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D20" si="1">D4/$I4</f>
+        <v>1.3777219430485763</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E20" si="2">E4/$J4</f>
+        <v>1.0086040837292924</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H20" si="3">H4/$H4</f>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I20" si="4">I4/$I4</f>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J20" si="5">J4/$J4</f>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M20" si="6">M4/$H4</f>
+        <v>1.0770975056689343</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14:N20" si="7">N4/$I4</f>
+        <v>3.0050251256281411</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14:O20" si="8">O4/$J4</f>
+        <v>0.9788108385771157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.55677655677655669</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1.1794117647058824</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.99854651162790709</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="6"/>
+        <v>1.0329670329670328</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="7"/>
+        <v>2.3455882352941173</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="8"/>
+        <v>0.9862579281183933</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.72631578947368425</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0.99890965732087234</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="6"/>
+        <v>0.99298245614035086</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="7"/>
+        <v>1.4514991181657848</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="8"/>
+        <v>1.0029595015576325</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.21886792452830187</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1.1451905626134302</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>1.2537659327925841</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="6"/>
+        <v>0.81132075471698117</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="7"/>
+        <v>3.9606775559588625</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="8"/>
+        <v>0.68945538818076479</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.67136150234741776</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1.1705069124423964</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>1.0419390650055507</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="6"/>
+        <v>1.1173708920187793</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="7"/>
+        <v>3.204301075268817</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="8"/>
+        <v>0.95177007524361679</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1.1864406779661016</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1.0065780818313379</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="6"/>
+        <v>1.1099999999999999</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="7"/>
+        <v>2.0435835351089588</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="8"/>
+        <v>0.98881726088672539</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.79411764705882348</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.99826224328593993</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="6"/>
+        <v>1.0588235294117645</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="7"/>
+        <v>0.98412698412698407</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="8"/>
+        <v>1.0082148499210111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="E3">
+        <v>14.013999999999999</v>
+      </c>
+      <c r="F3">
+        <v>13.739000000000001</v>
+      </c>
+      <c r="G3">
+        <v>14.962999999999999</v>
+      </c>
+      <c r="H3">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="I3">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="J3">
+        <v>14.035</v>
+      </c>
+      <c r="K3">
+        <v>13.911</v>
+      </c>
+      <c r="L3">
+        <v>14.326000000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.375</v>
+      </c>
+      <c r="N3">
+        <v>1.94</v>
+      </c>
+      <c r="O3">
+        <v>11.645</v>
+      </c>
+      <c r="P3">
+        <v>11.576000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>12.157999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.151</v>
+      </c>
+      <c r="D4">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E4">
+        <v>15.6</v>
+      </c>
+      <c r="F4">
+        <v>15.411</v>
+      </c>
+      <c r="G4">
+        <v>15.759</v>
+      </c>
+      <c r="H4">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="J4">
+        <v>15.436999999999999</v>
+      </c>
+      <c r="K4">
+        <v>15.372999999999999</v>
+      </c>
+      <c r="L4">
+        <v>15.718999999999999</v>
+      </c>
+      <c r="M4">
+        <v>0.3</v>
+      </c>
+      <c r="N4">
+        <v>2.254</v>
+      </c>
+      <c r="O4">
+        <v>15.121</v>
+      </c>
+      <c r="P4">
+        <v>14.959</v>
+      </c>
+      <c r="Q4">
+        <v>15.342000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.13</v>
+      </c>
+      <c r="D5">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E5">
+        <v>15.180999999999999</v>
+      </c>
+      <c r="F5">
+        <v>15.093999999999999</v>
+      </c>
+      <c r="G5">
+        <v>15.428000000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.185</v>
+      </c>
+      <c r="I5">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J5">
+        <v>15.064</v>
+      </c>
+      <c r="K5">
+        <v>14.993</v>
+      </c>
+      <c r="L5">
+        <v>15.249000000000001</v>
+      </c>
+      <c r="M5">
+        <v>0.188</v>
+      </c>
+      <c r="N5">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="O5">
+        <v>15.000999999999999</v>
+      </c>
+      <c r="P5">
+        <v>14.826000000000001</v>
+      </c>
+      <c r="Q5">
+        <v>15.356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>0.315</v>
+      </c>
+      <c r="C6">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.47</v>
+      </c>
+      <c r="E6">
+        <v>12.773</v>
+      </c>
+      <c r="F6">
+        <v>12.695</v>
+      </c>
+      <c r="G6">
+        <v>12.962999999999999</v>
+      </c>
+      <c r="H6">
+        <v>0.187</v>
+      </c>
+      <c r="I6">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="J6">
+        <v>12.771000000000001</v>
+      </c>
+      <c r="K6">
+        <v>12.696</v>
+      </c>
+      <c r="L6">
+        <v>12.976000000000001</v>
+      </c>
+      <c r="M6">
+        <v>0.191</v>
+      </c>
+      <c r="N6">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="O6">
+        <v>12.744</v>
+      </c>
+      <c r="P6">
+        <v>12.602</v>
+      </c>
+      <c r="Q6">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="C7">
+        <v>0.251</v>
+      </c>
+      <c r="D7">
+        <v>1.3240000000000001</v>
+      </c>
+      <c r="E7">
+        <v>1.38</v>
+      </c>
+      <c r="F7">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="G7">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="I7">
+        <v>1.1539999999999999</v>
+      </c>
+      <c r="J7">
+        <v>1.016</v>
+      </c>
+      <c r="K7">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="L7">
+        <v>1.071</v>
+      </c>
+      <c r="M7">
+        <v>0.99</v>
+      </c>
+      <c r="N7">
+        <v>5.45</v>
+      </c>
+      <c r="O7">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="P7">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="Q7">
+        <v>1.845</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.188</v>
+      </c>
+      <c r="C8">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="E8">
+        <v>16.401</v>
+      </c>
+      <c r="F8">
+        <v>15.973000000000001</v>
+      </c>
+      <c r="G8">
+        <v>16.544</v>
+      </c>
+      <c r="H8">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="I8">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="J8">
+        <v>15.973000000000001</v>
+      </c>
+      <c r="K8">
+        <v>15.817</v>
+      </c>
+      <c r="L8">
+        <v>16.145</v>
+      </c>
+      <c r="M8">
+        <v>0.224</v>
+      </c>
+      <c r="N8">
+        <v>2.0819999999999999</v>
+      </c>
+      <c r="O8">
+        <v>15.231</v>
+      </c>
+      <c r="P8">
+        <v>15.135</v>
+      </c>
+      <c r="Q8">
+        <v>15.332000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="C9">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E9">
+        <v>15.41</v>
+      </c>
+      <c r="F9">
+        <v>15.308999999999999</v>
+      </c>
+      <c r="G9">
+        <v>15.611000000000001</v>
+      </c>
+      <c r="H9">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="J9">
+        <v>15.404</v>
+      </c>
+      <c r="K9">
+        <v>15.157</v>
+      </c>
+      <c r="L9">
+        <v>15.792999999999999</v>
+      </c>
+      <c r="M9">
+        <v>0.105</v>
+      </c>
+      <c r="N9">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="O9">
+        <v>14.968</v>
+      </c>
+      <c r="P9">
+        <v>14.9</v>
+      </c>
+      <c r="Q9">
+        <v>15.292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C10">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E10">
+        <v>12.577999999999999</v>
+      </c>
+      <c r="F10">
+        <v>12.506</v>
+      </c>
+      <c r="G10">
+        <v>13.099</v>
+      </c>
+      <c r="H10">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.253</v>
+      </c>
+      <c r="J10">
+        <v>12.528</v>
+      </c>
+      <c r="K10">
+        <v>12.46</v>
+      </c>
+      <c r="L10">
+        <v>12.836</v>
+      </c>
+      <c r="M10">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="N10">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="O10">
+        <v>12.621</v>
+      </c>
+      <c r="P10">
+        <v>12.478999999999999</v>
+      </c>
+      <c r="Q10">
+        <v>12.759</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="E13">
+        <f>E3/$J3</f>
+        <v>0.99850374064837899</v>
+      </c>
+      <c r="J13">
+        <f>J3/$J3</f>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f>O3/$J3</f>
+        <v>0.8297114356964731</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="E14">
+        <f t="shared" ref="E14:E20" si="0">E4/$J4</f>
+        <v>1.0105590464468486</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J20" si="1">J4/$J4</f>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14:O20" si="2">O4/$J4</f>
+        <v>0.97952970136684592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1.0077668613913966</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>0.995817843866171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.0001566048077675</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>0.99788583509513729</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.3582677165354329</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>0.72145669291338577</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1.0267952169285668</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>0.95354660990421336</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.0003895092183848</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>0.97169566346403535</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.0039910600255426</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>1.0074233716475096</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
EXPRIMENTS - After specializing HashMap via LMS (with some level of inlining)
</commit_message>
<xml_diff>
--- a/docs/benchmarks/tpch_queries.xlsx
+++ b/docs/benchmarks/tpch_queries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tpch_standard" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="39">
   <si>
     <t>Dataset</t>
   </si>
@@ -134,6 +134,12 @@
   <si>
     <t>LMS-Inline-All</t>
   </si>
+  <si>
+    <t>LMS-Spec-Get</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
 </sst>
 </file>
 
@@ -184,8 +190,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -263,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -300,6 +326,16 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -336,6 +372,16 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,11 +695,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="172905096"/>
-        <c:axId val="172912040"/>
+        <c:axId val="162452008"/>
+        <c:axId val="162484328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172905096"/>
+        <c:axId val="162452008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172912040"/>
+        <c:crossAx val="162484328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -688,7 +734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172912040"/>
+        <c:axId val="162484328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172905096"/>
+        <c:crossAx val="162452008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1296,11 +1342,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="172293928"/>
-        <c:axId val="172297064"/>
+        <c:axId val="609027352"/>
+        <c:axId val="609030648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172293928"/>
+        <c:axId val="609027352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1355,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172297064"/>
+        <c:crossAx val="609030648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172297064"/>
+        <c:axId val="609030648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="19.0"/>
@@ -1329,7 +1375,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172293928"/>
+        <c:crossAx val="609027352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1426,28 +1472,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.02576</c:v>
+                  <c:v>1.080566323950784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.978810838577116</c:v>
+                  <c:v>1.028193713746122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.986257928118393</c:v>
+                  <c:v>1.120889022375732</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.002959501557632</c:v>
+                  <c:v>1.120605638705186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.689455388180765</c:v>
+                  <c:v>0.60528992878942</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.951770075243617</c:v>
+                  <c:v>0.957438888199529</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.988817260886725</c:v>
+                  <c:v>1.079264790350373</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.008214849921011</c:v>
+                  <c:v>1.132162497782508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,28 +1634,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.08112</c:v>
+                  <c:v>0.998651609640991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.008604083729292</c:v>
+                  <c:v>0.996492648050722</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.998546511627907</c:v>
+                  <c:v>1.00750863493017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.998909657320872</c:v>
+                  <c:v>1.004176818656457</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.253765932792584</c:v>
+                  <c:v>1.032553407934893</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.041939065005551</c:v>
+                  <c:v>1.030524879017248</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.006578081831338</c:v>
+                  <c:v>0.992245835726594</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99826224328594</c:v>
+                  <c:v>0.954763171899947</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Spec-Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$T$13:$T$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.088656666104837</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.982058545797923</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.085147920108124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.072050121823877</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.593082400813835</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92046159573148</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.040063182079265</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.077878304062445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,11 +1751,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="172338808"/>
-        <c:axId val="172341784"/>
+        <c:axId val="609101048"/>
+        <c:axId val="609104168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172338808"/>
+        <c:axId val="609101048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1764,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172341784"/>
+        <c:crossAx val="609104168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1645,7 +1772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172341784"/>
+        <c:axId val="609104168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1675,7 +1802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172338808"/>
+        <c:crossAx val="609101048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1782,28 +1909,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.953418027828191</c:v>
+                  <c:v>1.671345429647381</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.005025125628141</c:v>
+                  <c:v>2.449146757679181</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.345588235294117</c:v>
+                  <c:v>1.651138716356108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.451499118165785</c:v>
+                  <c:v>1.006112469437653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.960677555958862</c:v>
+                  <c:v>4.373413493653973</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.204301075268817</c:v>
+                  <c:v>2.240601503759398</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.043583535108959</c:v>
+                  <c:v>0.995283018867924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.984126984126984</c:v>
+                  <c:v>0.322916666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1944,28 +2071,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.813672111312765</c:v>
+                  <c:v>2.659020883259158</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.377721943048576</c:v>
+                  <c:v>1.581569965870307</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.179411764705882</c:v>
+                  <c:v>1.216356107660456</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.111111111111111</c:v>
+                  <c:v>1.077017114914425</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.14519056261343</c:v>
+                  <c:v>1.090848363393454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.170506912442396</c:v>
+                  <c:v>1.11922663802363</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.186440677966102</c:v>
+                  <c:v>1.093160377358491</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.166666666666666</c:v>
+                  <c:v>0.975260416666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Spec-Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$S$13:$S$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.216364258815474</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.603412969283276</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.742236024844721</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.007334963325183</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.852371409485638</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.561761546723952</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.10377358490566</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.424479166666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1980,11 +2188,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="611170040"/>
-        <c:axId val="611173416"/>
+        <c:axId val="609144584"/>
+        <c:axId val="609147704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="611170040"/>
+        <c:axId val="609144584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,7 +2201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611173416"/>
+        <c:crossAx val="609147704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2001,7 +2209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="611173416"/>
+        <c:axId val="609147704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2031,7 +2239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611170040"/>
+        <c:crossAx val="609144584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2138,28 +2346,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.481180811808118</c:v>
+                  <c:v>0.37129840546697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.077097505668934</c:v>
+                  <c:v>0.879629629629629</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.032967032967033</c:v>
+                  <c:v>1.110236220472441</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.992982456140351</c:v>
+                  <c:v>0.808571428571428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.811320754716981</c:v>
+                  <c:v>0.982632541133455</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.117370892018779</c:v>
+                  <c:v>0.689855072463768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.11</c:v>
+                  <c:v>0.680981595092024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.058823529411764</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2300,28 +2508,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.413284132841328</c:v>
+                  <c:v>0.33371298405467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.412698412698413</c:v>
+                  <c:v>0.253703703703704</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.556776556776557</c:v>
+                  <c:v>0.566929133858268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.726315789473684</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.218867924528302</c:v>
+                  <c:v>0.251371115173675</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.671361502347418</c:v>
+                  <c:v>0.455072463768116</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.417177914110429</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.794117647058823</c:v>
+                  <c:v>0.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_big!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Spec-Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_big!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_big!$R$13:$R$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.087699316628701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.262962962962963</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.696850393700787</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.257142857142857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.510968921389397</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.234782608695652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.061349693251534</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2336,11 +2625,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="611226392"/>
-        <c:axId val="611229368"/>
+        <c:axId val="609186824"/>
+        <c:axId val="609189944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="611226392"/>
+        <c:axId val="609186824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2349,7 +2638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611229368"/>
+        <c:crossAx val="609189944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2357,7 +2646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="611229368"/>
+        <c:axId val="609189944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611226392"/>
+        <c:crossAx val="609186824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2494,28 +2783,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.829711435696473</c:v>
+                  <c:v>0.865413198573127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.979529701366846</c:v>
+                  <c:v>1.069680249009621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.995817843866171</c:v>
+                  <c:v>1.176733605271415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.997885835095137</c:v>
+                  <c:v>1.154661592824137</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.721456692913386</c:v>
+                  <c:v>0.729353233830846</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.953546609904213</c:v>
+                  <c:v>0.986527624846169</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.971695663464035</c:v>
+                  <c:v>1.143380948743412</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.00742337164751</c:v>
+                  <c:v>1.178211351755041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2656,28 +2945,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.998503740648379</c:v>
+                  <c:v>1.100921521997622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.010559046446849</c:v>
+                  <c:v>0.997948500282965</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.007766861391397</c:v>
+                  <c:v>1.002431754000628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.000156604807767</c:v>
+                  <c:v>0.991845610220168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.358267716535433</c:v>
+                  <c:v>1.016915422885572</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.026795216928567</c:v>
+                  <c:v>1.022864175140877</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.000389509218385</c:v>
+                  <c:v>1.04002749980903</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.003991060025543</c:v>
+                  <c:v>0.969100074682599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tpch_bigdel!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LMS-Spec-Get</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>tpch_bigdel!$A$3:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>tpch1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tpch10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tpch12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tpch14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tpch2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tpch3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tpch4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tpch6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tpch_bigdel!$V$13:$V$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.780023781212842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.003112620260328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.053812362723564</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.050466612304068</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.647761194029851</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.899086728415053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.04132610190207</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.061799850634802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2692,11 +3062,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="611275368"/>
-        <c:axId val="611278344"/>
+        <c:axId val="608208872"/>
+        <c:axId val="608205736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="611275368"/>
+        <c:axId val="608208872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2705,7 +3075,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611278344"/>
+        <c:crossAx val="608205736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2713,7 +3083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="611278344"/>
+        <c:axId val="608205736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2752,7 +3122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="611275368"/>
+        <c:crossAx val="608208872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2957,16 +3327,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3314,7 +3684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
@@ -4375,7 +4745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
@@ -5674,15 +6044,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5698,8 +6071,11 @@
       <c r="M1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5713,7 +6089,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -5728,7 +6104,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
@@ -5751,8 +6127,23 @@
       <c r="Q2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5760,34 +6151,34 @@
         <v>0.47799999999999998</v>
       </c>
       <c r="C3">
-        <v>0.56000000000000005</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="D3">
-        <v>6.3040000000000003</v>
+        <v>7.7670000000000003</v>
       </c>
       <c r="E3">
-        <v>6.7569999999999997</v>
+        <v>5.9249999999999998</v>
       </c>
       <c r="F3">
-        <v>6.6749999999999998</v>
+        <v>5.8659999999999997</v>
       </c>
       <c r="G3">
-        <v>7.5129999999999999</v>
+        <v>5.9429999999999996</v>
       </c>
       <c r="H3">
-        <v>1.355</v>
+        <v>1.756</v>
       </c>
       <c r="I3">
-        <v>1.653</v>
+        <v>2.9209999999999998</v>
       </c>
       <c r="J3">
-        <v>6.25</v>
+        <v>5.9329999999999998</v>
       </c>
       <c r="K3">
-        <v>6.1779999999999999</v>
+        <v>5.8739999999999997</v>
       </c>
       <c r="L3">
-        <v>7.3179999999999996</v>
+        <v>5.968</v>
       </c>
       <c r="M3">
         <v>0.65200000000000002</v>
@@ -5804,8 +6195,23 @@
       <c r="Q3">
         <v>6.8179999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3">
+        <v>1.91</v>
+      </c>
+      <c r="S3">
+        <v>9.3949999999999996</v>
+      </c>
+      <c r="T3">
+        <v>6.4589999999999996</v>
+      </c>
+      <c r="U3">
+        <v>6.3520000000000003</v>
+      </c>
+      <c r="V3">
+        <v>7.0540000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -5813,34 +6219,34 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="C4">
-        <v>0.182</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="D4">
-        <v>1.645</v>
+        <v>2.3170000000000002</v>
       </c>
       <c r="E4">
-        <v>7.8540000000000001</v>
+        <v>7.3869999999999996</v>
       </c>
       <c r="F4">
-        <v>7.8049999999999997</v>
+        <v>7.2439999999999998</v>
       </c>
       <c r="G4">
-        <v>8.2949999999999999</v>
+        <v>7.4649999999999999</v>
       </c>
       <c r="H4">
-        <v>0.441</v>
+        <v>0.54</v>
       </c>
       <c r="I4">
-        <v>1.194</v>
+        <v>1.4650000000000001</v>
       </c>
       <c r="J4">
-        <v>7.7869999999999999</v>
+        <v>7.4130000000000003</v>
       </c>
       <c r="K4">
-        <v>7.6870000000000003</v>
+        <v>7.0810000000000004</v>
       </c>
       <c r="L4">
-        <v>7.9219999999999997</v>
+        <v>7.5049999999999999</v>
       </c>
       <c r="M4">
         <v>0.47499999999999998</v>
@@ -5857,8 +6263,23 @@
       <c r="Q4">
         <v>7.9779999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="S4">
+        <v>5.2789999999999999</v>
+      </c>
+      <c r="T4">
+        <v>7.28</v>
+      </c>
+      <c r="U4">
+        <v>7.1139999999999999</v>
+      </c>
+      <c r="V4">
+        <v>7.8689999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -5866,34 +6287,34 @@
         <v>0.182</v>
       </c>
       <c r="C5">
-        <v>0.152</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D5">
-        <v>0.80200000000000005</v>
+        <v>1.175</v>
       </c>
       <c r="E5">
-        <v>7.5570000000000004</v>
+        <v>6.7089999999999996</v>
       </c>
       <c r="F5">
-        <v>7.5119999999999996</v>
+        <v>6.6769999999999996</v>
       </c>
       <c r="G5">
-        <v>7.6219999999999999</v>
+        <v>6.7469999999999999</v>
       </c>
       <c r="H5">
-        <v>0.27300000000000002</v>
+        <v>0.254</v>
       </c>
       <c r="I5">
-        <v>0.68</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="J5">
-        <v>7.5679999999999996</v>
+        <v>6.6589999999999998</v>
       </c>
       <c r="K5">
-        <v>7.53</v>
+        <v>6.64</v>
       </c>
       <c r="L5">
-        <v>7.6319999999999997</v>
+        <v>6.7969999999999997</v>
       </c>
       <c r="M5">
         <v>0.28199999999999997</v>
@@ -5910,8 +6331,23 @@
       <c r="Q5">
         <v>7.4980000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="S5">
+        <v>1.6830000000000001</v>
+      </c>
+      <c r="T5">
+        <v>7.226</v>
+      </c>
+      <c r="U5">
+        <v>7.1879999999999997</v>
+      </c>
+      <c r="V5">
+        <v>7.3310000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -5919,34 +6355,34 @@
         <v>0.31</v>
       </c>
       <c r="C6">
-        <v>0.20699999999999999</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="D6">
-        <v>0.63</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="E6">
-        <v>6.4130000000000003</v>
+        <v>5.77</v>
       </c>
       <c r="F6">
-        <v>6.3639999999999999</v>
+        <v>5.694</v>
       </c>
       <c r="G6">
-        <v>6.4630000000000001</v>
+        <v>5.8079999999999998</v>
       </c>
       <c r="H6">
-        <v>0.28499999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="I6">
-        <v>0.56699999999999995</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="J6">
-        <v>6.42</v>
+        <v>5.7460000000000004</v>
       </c>
       <c r="K6">
-        <v>6.3949999999999996</v>
+        <v>5.67</v>
       </c>
       <c r="L6">
-        <v>6.4690000000000003</v>
+        <v>5.7750000000000004</v>
       </c>
       <c r="M6">
         <v>0.28299999999999997</v>
@@ -5963,8 +6399,23 @@
       <c r="Q6">
         <v>6.6139999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6">
+        <v>0.44</v>
+      </c>
+      <c r="S6">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="T6">
+        <v>6.16</v>
+      </c>
+      <c r="U6">
+        <v>6.13</v>
+      </c>
+      <c r="V6">
+        <v>6.3579999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5972,34 +6423,34 @@
         <v>0.84799999999999998</v>
       </c>
       <c r="C7">
-        <v>0.28999999999999998</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="D7">
-        <v>1.893</v>
+        <v>1.633</v>
       </c>
       <c r="E7">
-        <v>1.0820000000000001</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="F7">
-        <v>0.83499999999999996</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="G7">
-        <v>1.5780000000000001</v>
+        <v>1.3839999999999999</v>
       </c>
       <c r="H7">
-        <v>1.325</v>
+        <v>1.0940000000000001</v>
       </c>
       <c r="I7">
-        <v>1.653</v>
+        <v>1.4970000000000001</v>
       </c>
       <c r="J7">
-        <v>0.86299999999999999</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="K7">
-        <v>0.80500000000000005</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="L7">
-        <v>1.0620000000000001</v>
+        <v>1.405</v>
       </c>
       <c r="M7">
         <v>1.075</v>
@@ -6016,8 +6467,23 @@
       <c r="Q7">
         <v>1.732</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7">
+        <v>1.653</v>
+      </c>
+      <c r="S7">
+        <v>7.2640000000000002</v>
+      </c>
+      <c r="T7">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="U7">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="V7">
+        <v>1.7729999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -6025,34 +6491,34 @@
         <v>0.185</v>
       </c>
       <c r="C8">
-        <v>0.14299999999999999</v>
+        <v>0.157</v>
       </c>
       <c r="D8">
-        <v>0.76200000000000001</v>
+        <v>1.042</v>
       </c>
       <c r="E8">
-        <v>8.4469999999999992</v>
+        <v>8.3049999999999997</v>
       </c>
       <c r="F8">
-        <v>8.1</v>
+        <v>7.8470000000000004</v>
       </c>
       <c r="G8">
-        <v>8.6300000000000008</v>
+        <v>8.4540000000000006</v>
       </c>
       <c r="H8">
-        <v>0.21299999999999999</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="I8">
-        <v>0.65100000000000002</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="J8">
-        <v>8.1069999999999993</v>
+        <v>8.0589999999999993</v>
       </c>
       <c r="K8">
-        <v>8.0109999999999992</v>
+        <v>7.67</v>
       </c>
       <c r="L8">
-        <v>8.2859999999999996</v>
+        <v>8.39</v>
       </c>
       <c r="M8">
         <v>0.23799999999999999</v>
@@ -6069,8 +6535,23 @@
       <c r="Q8">
         <v>7.9329999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="S8">
+        <v>2.3849999999999998</v>
+      </c>
+      <c r="T8">
+        <v>7.4180000000000001</v>
+      </c>
+      <c r="U8">
+        <v>7.367</v>
+      </c>
+      <c r="V8">
+        <v>7.6749999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -6078,34 +6559,34 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="C9">
-        <v>0.06</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D9">
-        <v>0.49</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="E9">
-        <v>7.6509999999999998</v>
+        <v>6.91</v>
       </c>
       <c r="F9">
-        <v>7.569</v>
+        <v>6.8719999999999999</v>
       </c>
       <c r="G9">
-        <v>8.2210000000000001</v>
+        <v>6.944</v>
       </c>
       <c r="H9">
-        <v>0.1</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="I9">
-        <v>0.41299999999999998</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="J9">
-        <v>7.601</v>
+        <v>6.9640000000000004</v>
       </c>
       <c r="K9">
-        <v>7.5540000000000003</v>
+        <v>6.9089999999999998</v>
       </c>
       <c r="L9">
-        <v>7.79</v>
+        <v>7.0880000000000001</v>
       </c>
       <c r="M9">
         <v>0.111</v>
@@ -6122,8 +6603,23 @@
       <c r="Q9">
         <v>7.6719999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="S9">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="T9">
+        <v>7.2430000000000003</v>
+      </c>
+      <c r="U9">
+        <v>7.2229999999999999</v>
+      </c>
+      <c r="V9">
+        <v>7.5359999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -6131,34 +6627,34 @@
         <v>0.04</v>
       </c>
       <c r="C10">
-        <v>2.7E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="D10">
-        <v>0.29399999999999998</v>
+        <v>0.749</v>
       </c>
       <c r="E10">
-        <v>6.319</v>
+        <v>5.3819999999999997</v>
       </c>
       <c r="F10">
-        <v>6.2709999999999999</v>
+        <v>5.3559999999999999</v>
       </c>
       <c r="G10">
-        <v>6.5579999999999998</v>
+        <v>5.69</v>
       </c>
       <c r="H10">
-        <v>3.4000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I10">
-        <v>0.252</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="J10">
-        <v>6.33</v>
+        <v>5.6369999999999996</v>
       </c>
       <c r="K10">
-        <v>6.29</v>
+        <v>5.601</v>
       </c>
       <c r="L10">
-        <v>6.6109999999999998</v>
+        <v>5.6909999999999998</v>
       </c>
       <c r="M10">
         <v>3.5999999999999997E-2</v>
@@ -6175,19 +6671,34 @@
       <c r="Q10">
         <v>6.4619999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R10">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="S10">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="T10">
+        <v>6.0759999999999996</v>
+      </c>
+      <c r="U10">
+        <v>6.0419999999999998</v>
+      </c>
+      <c r="V10">
+        <v>6.2949999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="C13">
         <f>C3/$H3</f>
-        <v>0.41328413284132848</v>
+        <v>0.3337129840546697</v>
       </c>
       <c r="D13">
         <f>D3/$I3</f>
-        <v>3.8136721113127647</v>
+        <v>2.6590208832591582</v>
       </c>
       <c r="E13">
         <f>E3/$J3</f>
-        <v>1.0811199999999999</v>
+        <v>0.99865160964099109</v>
       </c>
       <c r="H13">
         <f>H3/$H3</f>
@@ -6203,29 +6714,41 @@
       </c>
       <c r="M13">
         <f>M3/$H3</f>
-        <v>0.48118081180811811</v>
+        <v>0.3712984054669704</v>
       </c>
       <c r="N13">
         <f>N3/$I3</f>
-        <v>2.953418027828191</v>
+        <v>1.6713454296473811</v>
       </c>
       <c r="O13">
         <f>O3/$J3</f>
-        <v>1.02576</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>1.0805663239507837</v>
+      </c>
+      <c r="R13">
+        <f>R3/$H3</f>
+        <v>1.0876993166287015</v>
+      </c>
+      <c r="S13">
+        <f>S3/$I3</f>
+        <v>3.2163642588154744</v>
+      </c>
+      <c r="T13">
+        <f>T3/$J3</f>
+        <v>1.0886566661048374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="C14">
         <f t="shared" ref="C14:C20" si="0">C4/$H4</f>
-        <v>0.41269841269841268</v>
+        <v>0.25370370370370371</v>
       </c>
       <c r="D14">
         <f t="shared" ref="D14:D20" si="1">D4/$I4</f>
-        <v>1.3777219430485763</v>
+        <v>1.5815699658703073</v>
       </c>
       <c r="E14">
         <f t="shared" ref="E14:E20" si="2">E4/$J4</f>
-        <v>1.0086040837292924</v>
+        <v>0.99649264805072157</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14:H20" si="3">H4/$H4</f>
@@ -6241,29 +6764,41 @@
       </c>
       <c r="M14">
         <f t="shared" ref="M14:M20" si="6">M4/$H4</f>
-        <v>1.0770975056689343</v>
+        <v>0.87962962962962954</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N20" si="7">N4/$I4</f>
-        <v>3.0050251256281411</v>
+        <v>2.449146757679181</v>
       </c>
       <c r="O14">
         <f t="shared" ref="O14:O20" si="8">O4/$J4</f>
-        <v>0.9788108385771157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>1.0281937137461217</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ref="R14:R20" si="9">R4/$H4</f>
+        <v>1.2629629629629631</v>
+      </c>
+      <c r="S14">
+        <f t="shared" ref="S14:S20" si="10">S4/$I4</f>
+        <v>3.6034129692832764</v>
+      </c>
+      <c r="T14">
+        <f t="shared" ref="T14:T20" si="11">T4/$J4</f>
+        <v>0.98205854579792262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.55677655677655669</v>
+        <v>0.56692913385826771</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>1.1794117647058824</v>
+        <v>1.2163561076604557</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>0.99854651162790709</v>
+        <v>1.0075086349301696</v>
       </c>
       <c r="H15">
         <f t="shared" si="3"/>
@@ -6279,29 +6814,41 @@
       </c>
       <c r="M15">
         <f t="shared" si="6"/>
-        <v>1.0329670329670328</v>
+        <v>1.1102362204724407</v>
       </c>
       <c r="N15">
         <f t="shared" si="7"/>
-        <v>2.3455882352941173</v>
+        <v>1.6511387163561078</v>
       </c>
       <c r="O15">
         <f t="shared" si="8"/>
-        <v>0.9862579281183933</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>1.1208890223757322</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="9"/>
+        <v>1.6968503937007873</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="10"/>
+        <v>1.7422360248447206</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="11"/>
+        <v>1.0851479201081244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.72631578947368425</v>
+        <v>0.48000000000000004</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>1.1111111111111112</v>
+        <v>1.0770171149144254</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>0.99890965732087234</v>
+        <v>1.0041768186564566</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
@@ -6317,29 +6864,41 @@
       </c>
       <c r="M16">
         <f t="shared" si="6"/>
-        <v>0.99298245614035086</v>
+        <v>0.8085714285714285</v>
       </c>
       <c r="N16">
         <f t="shared" si="7"/>
-        <v>1.4514991181657848</v>
+        <v>1.0061124694376529</v>
       </c>
       <c r="O16">
         <f t="shared" si="8"/>
-        <v>1.0029595015576325</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15">
+        <v>1.1206056387051861</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="9"/>
+        <v>1.2571428571428573</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="10"/>
+        <v>1.0073349633251834</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="11"/>
+        <v>1.0720501218238774</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20">
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.21886792452830187</v>
+        <v>0.25137111517367461</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>1.1451905626134302</v>
+        <v>1.0908483633934536</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>1.2537659327925841</v>
+        <v>1.032553407934893</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
@@ -6355,29 +6914,41 @@
       </c>
       <c r="M17">
         <f t="shared" si="6"/>
-        <v>0.81132075471698117</v>
+        <v>0.98263254113345511</v>
       </c>
       <c r="N17">
         <f t="shared" si="7"/>
-        <v>3.9606775559588625</v>
+        <v>4.3734134936539739</v>
       </c>
       <c r="O17">
         <f t="shared" si="8"/>
-        <v>0.68945538818076479</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15">
+        <v>0.60528992878942012</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="9"/>
+        <v>1.5109689213893966</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="10"/>
+        <v>4.8523714094856381</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="11"/>
+        <v>0.59308240081383512</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20">
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.67136150234741776</v>
+        <v>0.455072463768116</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>1.1705069124423964</v>
+        <v>1.1192266380236304</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>1.0419390650055507</v>
+        <v>1.0305248790172479</v>
       </c>
       <c r="H18">
         <f t="shared" si="3"/>
@@ -6393,29 +6964,41 @@
       </c>
       <c r="M18">
         <f t="shared" si="6"/>
-        <v>1.1173708920187793</v>
+        <v>0.68985507246376809</v>
       </c>
       <c r="N18">
         <f t="shared" si="7"/>
-        <v>3.204301075268817</v>
+        <v>2.240601503759398</v>
       </c>
       <c r="O18">
         <f t="shared" si="8"/>
-        <v>0.95177007524361679</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15">
+        <v>0.9574388881995286</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="9"/>
+        <v>1.2347826086956522</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="10"/>
+        <v>2.5617615467239525</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="11"/>
+        <v>0.92046159573148045</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.41717791411042948</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>1.1864406779661016</v>
+        <v>1.0931603773584906</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>1.0065780818313379</v>
+        <v>0.99224583572659386</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
@@ -6431,29 +7014,41 @@
       </c>
       <c r="M19">
         <f t="shared" si="6"/>
-        <v>1.1099999999999999</v>
+        <v>0.68098159509202449</v>
       </c>
       <c r="N19">
         <f t="shared" si="7"/>
-        <v>2.0435835351089588</v>
+        <v>0.99528301886792447</v>
       </c>
       <c r="O19">
         <f t="shared" si="8"/>
-        <v>0.98881726088672539</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15">
+        <v>1.0792647903503734</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="9"/>
+        <v>1.0613496932515336</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="10"/>
+        <v>1.1037735849056605</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="11"/>
+        <v>1.0400631820792647</v>
+      </c>
+    </row>
+    <row r="20" spans="3:20">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.79411764705882348</v>
+        <v>0.68</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>1.1666666666666665</v>
+        <v>0.97526041666666663</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>0.99826224328593993</v>
+        <v>0.95476317189994675</v>
       </c>
       <c r="H20">
         <f t="shared" si="3"/>
@@ -6469,15 +7064,27 @@
       </c>
       <c r="M20">
         <f t="shared" si="6"/>
-        <v>1.0588235294117645</v>
+        <v>0.71999999999999986</v>
       </c>
       <c r="N20">
         <f t="shared" si="7"/>
-        <v>0.98412698412698407</v>
+        <v>0.32291666666666669</v>
       </c>
       <c r="O20">
         <f t="shared" si="8"/>
-        <v>1.0082148499210111</v>
+        <v>1.1321624977825084</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="9"/>
+        <v>1.22</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="10"/>
+        <v>0.42447916666666669</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="11"/>
+        <v>1.0778783040624447</v>
       </c>
     </row>
   </sheetData>
@@ -6494,15 +7101,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6518,8 +7128,17 @@
       <c r="M1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6533,7 +7152,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -6548,7 +7167,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
@@ -6571,8 +7190,29 @@
       <c r="Q2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6580,34 +7220,34 @@
         <v>0.46899999999999997</v>
       </c>
       <c r="C3">
-        <v>0.23799999999999999</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="D3">
-        <v>0.45800000000000002</v>
+        <v>7.7670000000000003</v>
       </c>
       <c r="E3">
-        <v>14.013999999999999</v>
+        <v>14.814</v>
       </c>
       <c r="F3">
-        <v>13.739000000000001</v>
+        <v>14.042999999999999</v>
       </c>
       <c r="G3">
-        <v>14.962999999999999</v>
+        <v>15.146000000000001</v>
       </c>
       <c r="H3">
-        <v>0.34200000000000003</v>
+        <v>1.756</v>
       </c>
       <c r="I3">
-        <v>0.45800000000000002</v>
+        <v>2.9209999999999998</v>
       </c>
       <c r="J3">
-        <v>14.035</v>
+        <v>13.456</v>
       </c>
       <c r="K3">
-        <v>13.911</v>
+        <v>13.093</v>
       </c>
       <c r="L3">
-        <v>14.326000000000001</v>
+        <v>13.818</v>
       </c>
       <c r="M3">
         <v>0.375</v>
@@ -6624,8 +7264,29 @@
       <c r="Q3">
         <v>12.157999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="T3">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="U3">
+        <v>1.5940000000000001</v>
+      </c>
+      <c r="V3">
+        <v>10.496</v>
+      </c>
+      <c r="W3">
+        <v>10.345000000000001</v>
+      </c>
+      <c r="X3">
+        <v>11.427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -6633,34 +7294,34 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="C4">
-        <v>0.151</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="D4">
-        <v>0.81399999999999995</v>
+        <v>2.3170000000000002</v>
       </c>
       <c r="E4">
-        <v>15.6</v>
+        <v>14.106999999999999</v>
       </c>
       <c r="F4">
-        <v>15.411</v>
+        <v>14.007999999999999</v>
       </c>
       <c r="G4">
-        <v>15.759</v>
+        <v>14.343999999999999</v>
       </c>
       <c r="H4">
-        <v>0.26300000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="I4">
-        <v>0.66100000000000003</v>
+        <v>1.4650000000000001</v>
       </c>
       <c r="J4">
-        <v>15.436999999999999</v>
+        <v>14.135999999999999</v>
       </c>
       <c r="K4">
-        <v>15.372999999999999</v>
+        <v>14.057</v>
       </c>
       <c r="L4">
-        <v>15.718999999999999</v>
+        <v>14.382</v>
       </c>
       <c r="M4">
         <v>0.3</v>
@@ -6677,8 +7338,29 @@
       <c r="Q4">
         <v>15.342000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4">
+        <v>0.23</v>
+      </c>
+      <c r="T4">
+        <v>1.738</v>
+      </c>
+      <c r="U4">
+        <v>11.362</v>
+      </c>
+      <c r="V4">
+        <v>14.18</v>
+      </c>
+      <c r="W4">
+        <v>13.926</v>
+      </c>
+      <c r="X4">
+        <v>15.103999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -6686,34 +7368,34 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="C5">
-        <v>0.13</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D5">
-        <v>0.58399999999999996</v>
+        <v>1.175</v>
       </c>
       <c r="E5">
-        <v>15.180999999999999</v>
+        <v>12.779</v>
       </c>
       <c r="F5">
-        <v>15.093999999999999</v>
+        <v>12.67</v>
       </c>
       <c r="G5">
-        <v>15.428000000000001</v>
+        <v>12.906000000000001</v>
       </c>
       <c r="H5">
-        <v>0.185</v>
+        <v>0.254</v>
       </c>
       <c r="I5">
-        <v>0.46400000000000002</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="J5">
-        <v>15.064</v>
+        <v>12.747999999999999</v>
       </c>
       <c r="K5">
-        <v>14.993</v>
+        <v>12.538</v>
       </c>
       <c r="L5">
-        <v>15.249000000000001</v>
+        <v>12.8</v>
       </c>
       <c r="M5">
         <v>0.188</v>
@@ -6730,8 +7412,29 @@
       <c r="Q5">
         <v>15.356</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5">
+        <v>0.184</v>
+      </c>
+      <c r="T5">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="U5">
+        <v>2.75</v>
+      </c>
+      <c r="V5">
+        <v>13.433999999999999</v>
+      </c>
+      <c r="W5">
+        <v>13.186999999999999</v>
+      </c>
+      <c r="X5">
+        <v>13.705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -6739,34 +7442,34 @@
         <v>0.315</v>
       </c>
       <c r="C6">
-        <v>0.16700000000000001</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="D6">
-        <v>0.47</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="E6">
-        <v>12.773</v>
+        <v>10.946999999999999</v>
       </c>
       <c r="F6">
-        <v>12.695</v>
+        <v>10.858000000000001</v>
       </c>
       <c r="G6">
-        <v>12.962999999999999</v>
+        <v>11.045</v>
       </c>
       <c r="H6">
-        <v>0.187</v>
+        <v>0.35</v>
       </c>
       <c r="I6">
-        <v>0.39200000000000002</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="J6">
-        <v>12.771000000000001</v>
+        <v>11.037000000000001</v>
       </c>
       <c r="K6">
-        <v>12.696</v>
+        <v>10.888</v>
       </c>
       <c r="L6">
-        <v>12.976000000000001</v>
+        <v>11.103999999999999</v>
       </c>
       <c r="M6">
         <v>0.191</v>
@@ -6783,8 +7486,29 @@
       <c r="Q6">
         <v>13.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="T6">
+        <v>0.505</v>
+      </c>
+      <c r="U6">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="V6">
+        <v>11.593999999999999</v>
+      </c>
+      <c r="W6">
+        <v>11.483000000000001</v>
+      </c>
+      <c r="X6">
+        <v>11.741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -6792,31 +7516,31 @@
         <v>0.83199999999999996</v>
       </c>
       <c r="C7">
-        <v>0.251</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="D7">
-        <v>1.3240000000000001</v>
+        <v>1.633</v>
       </c>
       <c r="E7">
-        <v>1.38</v>
+        <v>1.022</v>
       </c>
       <c r="F7">
-        <v>0.86499999999999999</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="G7">
-        <v>1.6519999999999999</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="H7">
-        <v>0.85599999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
       <c r="I7">
-        <v>1.1539999999999999</v>
+        <v>1.4970000000000001</v>
       </c>
       <c r="J7">
-        <v>1.016</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="K7">
-        <v>0.93899999999999995</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="L7">
         <v>1.071</v>
@@ -6836,8 +7560,29 @@
       <c r="Q7">
         <v>1.845</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S7">
+        <v>0.872</v>
+      </c>
+      <c r="T7">
+        <v>1.762</v>
+      </c>
+      <c r="U7">
+        <v>8.2739999999999991</v>
+      </c>
+      <c r="V7">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="W7">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="X7">
+        <v>1.8540000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -6845,34 +7590,34 @@
         <v>0.188</v>
       </c>
       <c r="C8">
-        <v>0.13600000000000001</v>
+        <v>0.157</v>
       </c>
       <c r="D8">
-        <v>0.74299999999999999</v>
+        <v>1.042</v>
       </c>
       <c r="E8">
-        <v>16.401</v>
+        <v>15.792</v>
       </c>
       <c r="F8">
+        <v>15.554</v>
+      </c>
+      <c r="G8">
         <v>15.973000000000001</v>
       </c>
-      <c r="G8">
-        <v>16.544</v>
-      </c>
       <c r="H8">
-        <v>0.19900000000000001</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="I8">
-        <v>0.57199999999999995</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="J8">
-        <v>15.973000000000001</v>
+        <v>15.439</v>
       </c>
       <c r="K8">
-        <v>15.817</v>
+        <v>15.284000000000001</v>
       </c>
       <c r="L8">
-        <v>16.145</v>
+        <v>15.603999999999999</v>
       </c>
       <c r="M8">
         <v>0.224</v>
@@ -6889,8 +7634,29 @@
       <c r="Q8">
         <v>15.332000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" t="s">
+        <v>11</v>
+      </c>
+      <c r="S8">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="T8">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="U8">
+        <v>2.5419999999999998</v>
+      </c>
+      <c r="V8">
+        <v>13.881</v>
+      </c>
+      <c r="W8">
+        <v>13.616</v>
+      </c>
+      <c r="X8">
+        <v>14.082000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -6898,34 +7664,34 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="C9">
-        <v>5.8000000000000003E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D9">
-        <v>0.46500000000000002</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="E9">
-        <v>15.41</v>
+        <v>13.615</v>
       </c>
       <c r="F9">
-        <v>15.308999999999999</v>
+        <v>13.189</v>
       </c>
       <c r="G9">
-        <v>15.611000000000001</v>
+        <v>13.724</v>
       </c>
       <c r="H9">
-        <v>9.5000000000000001E-2</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="I9">
-        <v>0.41599999999999998</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="J9">
-        <v>15.404</v>
+        <v>13.090999999999999</v>
       </c>
       <c r="K9">
-        <v>15.157</v>
+        <v>12.93</v>
       </c>
       <c r="L9">
-        <v>15.792999999999999</v>
+        <v>13.3</v>
       </c>
       <c r="M9">
         <v>0.105</v>
@@ -6942,8 +7708,29 @@
       <c r="Q9">
         <v>15.292</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T9">
+        <v>0.182</v>
+      </c>
+      <c r="U9">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="V9">
+        <v>13.632</v>
+      </c>
+      <c r="W9">
+        <v>13.529</v>
+      </c>
+      <c r="X9">
+        <v>14.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -6951,34 +7738,34 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C10">
-        <v>2.8000000000000001E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="D10">
-        <v>0.30499999999999999</v>
+        <v>0.749</v>
       </c>
       <c r="E10">
-        <v>12.577999999999999</v>
+        <v>10.381</v>
       </c>
       <c r="F10">
-        <v>12.506</v>
+        <v>10.324</v>
       </c>
       <c r="G10">
-        <v>13.099</v>
+        <v>10.414</v>
       </c>
       <c r="H10">
-        <v>3.4000000000000002E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I10">
-        <v>0.253</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="J10">
-        <v>12.528</v>
+        <v>10.712</v>
       </c>
       <c r="K10">
-        <v>12.46</v>
+        <v>10.659000000000001</v>
       </c>
       <c r="L10">
-        <v>12.836</v>
+        <v>10.739000000000001</v>
       </c>
       <c r="M10">
         <v>3.5999999999999997E-2</v>
@@ -6995,11 +7782,32 @@
       <c r="Q10">
         <v>12.759</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10">
+        <v>3.9E-2</v>
+      </c>
+      <c r="T10">
+        <v>6.3E-2</v>
+      </c>
+      <c r="U10">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="V10">
+        <v>11.374000000000001</v>
+      </c>
+      <c r="W10">
+        <v>11.294</v>
+      </c>
+      <c r="X10">
+        <v>11.683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="E13">
         <f>E3/$J3</f>
-        <v>0.99850374064837899</v>
+        <v>1.1009215219976218</v>
       </c>
       <c r="J13">
         <f>J3/$J3</f>
@@ -7007,13 +7815,17 @@
       </c>
       <c r="O13">
         <f>O3/$J3</f>
-        <v>0.8297114356964731</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>0.86541319857312726</v>
+      </c>
+      <c r="V13">
+        <f>V3/$J3</f>
+        <v>0.78002378121284188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="E14">
         <f t="shared" ref="E14:E20" si="0">E4/$J4</f>
-        <v>1.0105590464468486</v>
+        <v>0.99794850028296544</v>
       </c>
       <c r="J14">
         <f t="shared" ref="J14:J20" si="1">J4/$J4</f>
@@ -7021,13 +7833,17 @@
       </c>
       <c r="O14">
         <f t="shared" ref="O14:O20" si="2">O4/$J4</f>
-        <v>0.97952970136684592</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>1.0696802490096209</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ref="V14:V20" si="3">V4/$J4</f>
+        <v>1.0031126202603282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1.0077668613913966</v>
+        <v>1.0024317540006276</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
@@ -7035,13 +7851,17 @@
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
-        <v>0.995817843866171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>1.1767336052714152</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="3"/>
+        <v>1.0538123627235645</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1.0001566048077675</v>
+        <v>0.99184561022016837</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
@@ -7049,13 +7869,17 @@
       </c>
       <c r="O16">
         <f t="shared" si="2"/>
-        <v>0.99788583509513729</v>
-      </c>
-    </row>
-    <row r="17" spans="5:15">
+        <v>1.1546615928241368</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="3"/>
+        <v>1.050466612304068</v>
+      </c>
+    </row>
+    <row r="17" spans="5:22">
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1.3582677165354329</v>
+        <v>1.0169154228855724</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
@@ -7063,13 +7887,17 @@
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
-        <v>0.72145669291338577</v>
-      </c>
-    </row>
-    <row r="18" spans="5:15">
+        <v>0.72935323383084583</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="3"/>
+        <v>0.64776119402985088</v>
+      </c>
+    </row>
+    <row r="18" spans="5:22">
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>1.0267952169285668</v>
+        <v>1.0228641751408769</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
@@ -7077,13 +7905,17 @@
       </c>
       <c r="O18">
         <f t="shared" si="2"/>
-        <v>0.95354660990421336</v>
-      </c>
-    </row>
-    <row r="19" spans="5:15">
+        <v>0.98652762484616874</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="3"/>
+        <v>0.89908672841505277</v>
+      </c>
+    </row>
+    <row r="19" spans="5:22">
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1.0003895092183848</v>
+        <v>1.0400274998090291</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
@@ -7091,13 +7923,17 @@
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>0.97169566346403535</v>
-      </c>
-    </row>
-    <row r="20" spans="5:15">
+        <v>1.1433809487434117</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="3"/>
+        <v>1.0413261019020701</v>
+      </c>
+    </row>
+    <row r="20" spans="5:22">
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>1.0039910600255426</v>
+        <v>0.96910007468259896</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
@@ -7105,7 +7941,21 @@
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
-        <v>1.0074233716475096</v>
+        <v>1.1782113517550412</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="3"/>
+        <v>1.0617998506348021</v>
+      </c>
+    </row>
+    <row r="23" spans="5:22">
+      <c r="O23">
+        <f>AVERAGE(O13:O20)</f>
+        <v>1.0379952256067209</v>
+      </c>
+      <c r="V23">
+        <f>AVERAGE(V13:V20)</f>
+        <v>0.94217365643532247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>